<commit_message>
fix: jadwal, absensi, and meeting
</commit_message>
<xml_diff>
--- a/prisma/seeds/data/matakuliah.xlsx
+++ b/prisma/seeds/data/matakuliah.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="221">
   <si>
     <t>KODE</t>
   </si>
@@ -31,6 +31,9 @@
     <t>BIDANG_MINAT</t>
   </si>
   <si>
+    <t>IS_TEORI</t>
+  </si>
+  <si>
     <t>SINF1001</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>RPL</t>
   </si>
   <si>
+    <t>TEORI</t>
+  </si>
+  <si>
     <t>SINF1002</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t>PRAKTIKUM PEMROGRAMAN</t>
   </si>
   <si>
+    <t>PRAKTIKUM</t>
+  </si>
+  <si>
     <t>SINF1004</t>
   </si>
   <si>
@@ -665,78 +674,6 @@
   </si>
   <si>
     <t>PRAKTIKUM KEWIRAUSAHAAN</t>
-  </si>
-  <si>
-    <t>MKWUP001</t>
-  </si>
-  <si>
-    <t>KULIAH KERJA NYATA</t>
-  </si>
-  <si>
-    <t>SMPA6001</t>
-  </si>
-  <si>
-    <t>PRAKTIK WIRAUSAHA</t>
-  </si>
-  <si>
-    <t>SMPA6002</t>
-  </si>
-  <si>
-    <t>PUBLIKASI ILMIAH</t>
-  </si>
-  <si>
-    <t>SMPA6003</t>
-  </si>
-  <si>
-    <t>MAGANG INDUTRI A</t>
-  </si>
-  <si>
-    <t>SMPA6004</t>
-  </si>
-  <si>
-    <t>MAGANG INDUSTRI B</t>
-  </si>
-  <si>
-    <t>SMPA6005</t>
-  </si>
-  <si>
-    <t>PROYEK DESA A</t>
-  </si>
-  <si>
-    <t>SMPA6006</t>
-  </si>
-  <si>
-    <t>PROYEK DESA B</t>
-  </si>
-  <si>
-    <t>SMPA6007</t>
-  </si>
-  <si>
-    <t>PRAKTIK PEMBELAJARAN SAINS A</t>
-  </si>
-  <si>
-    <t>SMPA6008</t>
-  </si>
-  <si>
-    <t>PRAKTIK PEMBELAJARAN SAINS B</t>
-  </si>
-  <si>
-    <t>SMPAP001</t>
-  </si>
-  <si>
-    <t>KULIAH KERJA PRAKTIK</t>
-  </si>
-  <si>
-    <t>SMPAP002</t>
-  </si>
-  <si>
-    <t>PROPOSAL PENELITIAN</t>
-  </si>
-  <si>
-    <t>SMPAPA01</t>
-  </si>
-  <si>
-    <t>TUGAS AKHIR</t>
   </si>
 </sst>
 </file>
@@ -779,18 +716,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1022,7 +953,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1037,2306 +968,2474 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>3.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
         <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>3.0</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
         <v>1.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>1.0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
         <v>2.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>2.0</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
         <v>1.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>1.0</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
         <v>2.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>1.0</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
         <v>2.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>2.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1">
         <v>2.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <v>1.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1">
         <v>2.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>2.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
         <v>2.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
         <v>1.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="2">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1">
         <v>3.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1">
         <v>2.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1">
         <v>3.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <v>1.0</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>12</v>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1">
         <v>3.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>2.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="2">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
         <v>3.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1">
         <v>1.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1">
         <v>3.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
         <v>2.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="2">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1">
         <v>4.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
         <v>2.0</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>12</v>
+      <c r="F17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="2">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1">
         <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1">
         <v>1.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1">
         <v>4.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1">
         <v>2.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="2">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1">
         <v>3.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1">
         <v>2.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="2">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1">
         <v>4.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1">
         <v>2.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="2">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1">
         <v>3.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1">
         <v>1.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="2">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1">
         <v>4.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1">
         <v>1.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="2">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1">
         <v>3.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1">
         <v>2.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="2">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1">
         <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1">
         <v>2.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="2">
+        <v>62</v>
+      </c>
+      <c r="B26" s="1">
         <v>3.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1">
         <v>1.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>58</v>
+      <c r="G27" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="2">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1">
         <v>3.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1">
         <v>2.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2">
+        <v>68</v>
+      </c>
+      <c r="B29" s="1">
         <v>4.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1">
         <v>2.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="2">
+        <v>70</v>
+      </c>
+      <c r="B30" s="1">
         <v>3.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1">
         <v>1.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="2">
+        <v>72</v>
+      </c>
+      <c r="B31" s="1">
         <v>4.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="1">
         <v>1.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="2">
+        <v>74</v>
+      </c>
+      <c r="B32" s="1">
         <v>4.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1">
         <v>2.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="2">
+        <v>76</v>
+      </c>
+      <c r="B33" s="1">
         <v>4.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1">
         <v>1.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="2">
+        <v>78</v>
+      </c>
+      <c r="B34" s="1">
         <v>4.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1">
         <v>2.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" s="2">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1">
         <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1">
         <v>1.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>77</v>
+      <c r="G36" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="2">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1">
         <v>5.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1">
         <v>1.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="2">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1">
         <v>5.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
         <v>2.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="2">
+        <v>89</v>
+      </c>
+      <c r="B39" s="1">
         <v>5.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E39" s="1">
         <v>1.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="2">
+        <v>91</v>
+      </c>
+      <c r="B40" s="1">
         <v>5.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E40" s="1">
         <v>2.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="2">
+        <v>93</v>
+      </c>
+      <c r="B41" s="1">
         <v>6.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1">
         <v>2.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="2">
+        <v>95</v>
+      </c>
+      <c r="B42" s="1">
         <v>5.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E42" s="1">
         <v>1.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B43" s="2">
+        <v>97</v>
+      </c>
+      <c r="B43" s="1">
         <v>6.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1">
         <v>2.0</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>12</v>
+      <c r="F43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="2">
+        <v>99</v>
+      </c>
+      <c r="B44" s="1">
         <v>6.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1">
         <v>2.0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" s="2">
+        <v>101</v>
+      </c>
+      <c r="B45" s="1">
         <v>6.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1">
         <v>1.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="2">
+        <v>103</v>
+      </c>
+      <c r="B46" s="1">
         <v>6.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E46" s="1">
         <v>2.0</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>12</v>
+      <c r="F46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47" s="2">
+        <v>105</v>
+      </c>
+      <c r="B47" s="1">
         <v>7.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E47" s="1">
         <v>2.0</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>12</v>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="2">
+        <v>107</v>
+      </c>
+      <c r="B48" s="1">
         <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E48" s="1">
         <v>2.0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="2">
+        <v>110</v>
+      </c>
+      <c r="B49" s="1">
         <v>5.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E49" s="1">
         <v>1.0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="2">
+        <v>112</v>
+      </c>
+      <c r="B50" s="1">
         <v>5.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E50" s="1">
         <v>2.0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="2">
+        <v>114</v>
+      </c>
+      <c r="B51" s="1">
         <v>6.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E51" s="1">
         <v>2.0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="2">
+        <v>116</v>
+      </c>
+      <c r="B52" s="1">
         <v>5.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E52" s="1">
         <v>1.0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" s="2">
+        <v>118</v>
+      </c>
+      <c r="B53" s="1">
         <v>6.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E53" s="1">
         <v>1.0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="2">
+        <v>120</v>
+      </c>
+      <c r="B54" s="1">
         <v>5.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E54" s="1">
         <v>2.0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B55" s="2">
+        <v>122</v>
+      </c>
+      <c r="B55" s="1">
         <v>6.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E55" s="1">
         <v>2.0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="2">
+        <v>124</v>
+      </c>
+      <c r="B56" s="1">
         <v>5.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E56" s="1">
         <v>1.0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57" s="2">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1">
         <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E57" s="1">
         <v>1.0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" s="2">
+        <v>128</v>
+      </c>
+      <c r="B58" s="1">
         <v>5.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E58" s="1">
         <v>2.0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="2">
+        <v>130</v>
+      </c>
+      <c r="B59" s="1">
         <v>6.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E59" s="1">
         <v>2.0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B60" s="2">
+        <v>132</v>
+      </c>
+      <c r="B60" s="1">
         <v>5.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E60" s="1">
         <v>1.0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="2">
+        <v>134</v>
+      </c>
+      <c r="B61" s="1">
         <v>6.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E61" s="1">
         <v>1.0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B62" s="2">
+        <v>136</v>
+      </c>
+      <c r="B62" s="1">
         <v>5.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E62" s="1">
         <v>2.0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B63" s="2">
+        <v>138</v>
+      </c>
+      <c r="B63" s="1">
         <v>6.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E63" s="1">
         <v>2.0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B64" s="2">
+        <v>140</v>
+      </c>
+      <c r="B64" s="1">
         <v>5.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E64" s="1">
         <v>1.0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B65" s="2">
+        <v>142</v>
+      </c>
+      <c r="B65" s="1">
         <v>6.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E65" s="1">
         <v>1.0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B66" s="2">
+        <v>144</v>
+      </c>
+      <c r="B66" s="1">
         <v>5.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E66" s="1">
         <v>2.0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B67" s="2">
+        <v>146</v>
+      </c>
+      <c r="B67" s="1">
         <v>6.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E67" s="1">
         <v>2.0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B68" s="2">
+        <v>148</v>
+      </c>
+      <c r="B68" s="1">
         <v>5.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E68" s="1">
         <v>1.0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B69" s="2">
+        <v>150</v>
+      </c>
+      <c r="B69" s="1">
         <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E69" s="1">
         <v>1.0</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B70" s="2">
+        <v>152</v>
+      </c>
+      <c r="B70" s="1">
         <v>5.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E70" s="1">
         <v>2.0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="2">
+        <v>154</v>
+      </c>
+      <c r="B71" s="1">
         <v>6.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E71" s="1">
         <v>2.0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B72" s="2">
+        <v>156</v>
+      </c>
+      <c r="B72" s="1">
         <v>5.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E72" s="1">
         <v>1.0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B73" s="2">
+        <v>158</v>
+      </c>
+      <c r="B73" s="1">
         <v>6.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E73" s="1">
         <v>1.0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B74" s="4">
+        <v>160</v>
+      </c>
+      <c r="B74" s="3">
         <v>7.0</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>158</v>
+      <c r="C74" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E74" s="1">
         <v>2.0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="2">
+        <v>162</v>
+      </c>
+      <c r="B75" s="1">
         <v>6.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E75" s="1">
         <v>2.0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B76" s="2">
+        <v>164</v>
+      </c>
+      <c r="B76" s="1">
         <v>7.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E76" s="1">
         <v>1.0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B77" s="2">
+        <v>166</v>
+      </c>
+      <c r="B77" s="1">
         <v>6.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E77" s="1">
         <v>1.0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B78" s="2">
+        <v>167</v>
+      </c>
+      <c r="B78" s="1">
         <v>7.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E78" s="1">
         <v>2.0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B79" s="2">
+        <v>169</v>
+      </c>
+      <c r="B79" s="1">
         <v>6.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E79" s="1">
         <v>2.0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="4">
+        <v>171</v>
+      </c>
+      <c r="B80" s="3">
         <v>7.0</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>169</v>
+      <c r="C80" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E80" s="1">
         <v>1.0</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B81" s="2">
+        <v>173</v>
+      </c>
+      <c r="B81" s="1">
         <v>6.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E81" s="1">
         <v>1.0</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B82" s="2">
+        <v>175</v>
+      </c>
+      <c r="B82" s="1">
         <v>7.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E82" s="1">
         <v>2.0</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B83" s="2">
+        <v>177</v>
+      </c>
+      <c r="B83" s="1">
         <v>6.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E83" s="1">
         <v>2.0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B84" s="2">
+        <v>179</v>
+      </c>
+      <c r="B84" s="1">
         <v>7.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E84" s="1">
         <v>1.0</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B85" s="2">
+        <v>181</v>
+      </c>
+      <c r="B85" s="1">
         <v>6.0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E85" s="1">
         <v>1.0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B86" s="2">
+        <v>183</v>
+      </c>
+      <c r="B86" s="1">
         <v>7.0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E86" s="1">
         <v>2.0</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B87" s="2">
+        <v>185</v>
+      </c>
+      <c r="B87" s="1">
         <v>6.0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E87" s="1">
         <v>2.0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B88" s="2">
+        <v>187</v>
+      </c>
+      <c r="B88" s="1">
         <v>7.0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E88" s="1">
         <v>1.0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B89" s="2">
+        <v>189</v>
+      </c>
+      <c r="B89" s="1">
         <v>6.0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E89" s="1">
         <v>1.0</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B90" s="2">
+        <v>191</v>
+      </c>
+      <c r="B90" s="1">
         <v>7.0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E90" s="1">
         <v>2.0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B91" s="2">
+        <v>193</v>
+      </c>
+      <c r="B91" s="1">
         <v>6.0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E91" s="1">
         <v>2.0</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B92" s="2">
+        <v>195</v>
+      </c>
+      <c r="B92" s="1">
         <v>7.0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E92" s="1">
         <v>1.0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B93" s="2">
+        <v>197</v>
+      </c>
+      <c r="B93" s="1">
         <v>6.0</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E93" s="1">
         <v>1.0</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B94" s="2">
+        <v>199</v>
+      </c>
+      <c r="B94" s="1">
         <v>7.0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E94" s="1">
         <v>11.0</v>
       </c>
-      <c r="F94" s="3" t="s">
-        <v>12</v>
+      <c r="F94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B95" s="2">
+        <v>201</v>
+      </c>
+      <c r="B95" s="1">
         <v>6.0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E95" s="1">
         <v>2.0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B96" s="2">
+        <v>203</v>
+      </c>
+      <c r="B96" s="1">
         <v>7.0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E96" s="1">
         <v>1.0</v>
       </c>
-      <c r="F96" s="3" t="s">
-        <v>12</v>
+      <c r="F96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B97" s="2">
+        <v>205</v>
+      </c>
+      <c r="B97" s="1">
         <v>6.0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E97" s="1">
         <v>1.0</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B98" s="4">
+        <v>207</v>
+      </c>
+      <c r="B98" s="3">
         <v>7.0</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>205</v>
+      <c r="C98" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E98" s="1">
         <v>1.0</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>12</v>
+      <c r="F98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B99" s="2">
+        <v>209</v>
+      </c>
+      <c r="B99" s="1">
         <v>6.0</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E99" s="1">
         <v>2.0</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>12</v>
+      <c r="F99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B100" s="2">
+        <v>211</v>
+      </c>
+      <c r="B100" s="1">
         <v>7.0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E100" s="1">
         <v>1.0</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>12</v>
+      <c r="F100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B101" s="2">
+        <v>213</v>
+      </c>
+      <c r="B101" s="1">
         <v>6.0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E101" s="1">
         <v>2.0</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>12</v>
+      <c r="F101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B102" s="2">
+        <v>215</v>
+      </c>
+      <c r="B102" s="1">
         <v>7.0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E102" s="1">
         <v>1.0</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>12</v>
+      <c r="F102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B103" s="2">
+        <v>217</v>
+      </c>
+      <c r="B103" s="1">
         <v>5.0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E103" s="1">
         <v>2.0</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>12</v>
+      <c r="F103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B104" s="2">
+        <v>219</v>
+      </c>
+      <c r="B104" s="1">
         <v>5.0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E104" s="1">
         <v>1.0</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>12</v>
+      <c r="F104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B105" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B106" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E106" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B107" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E107" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B108" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E108" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B109" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E109" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B110" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E110" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B111" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E111" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B112" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E112" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B113" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E113" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B114" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B115" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B116" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
     </row>
     <row r="117" ht="15.75" customHeight="1"/>
     <row r="118" ht="15.75" customHeight="1"/>

</xml_diff>